<commit_message>
diff column added to Stock reporter
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Total gain (%)</t>
         </is>
       </c>
@@ -469,6 +474,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>52.07</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>43.27 %</t>
         </is>
       </c>
@@ -487,6 +497,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>19.12</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>22.60 %</t>
         </is>
       </c>
@@ -505,6 +520,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>79.57</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>99.66 %</t>
         </is>
       </c>
@@ -523,6 +543,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>45.34</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>30.65 %</t>
         </is>
       </c>
@@ -541,6 +566,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>15.15</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>52.31 %</t>
         </is>
       </c>
@@ -559,6 +589,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>1632.62</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>3.64 %</t>
         </is>
       </c>
@@ -577,6 +612,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>87.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>12.10 %</t>
         </is>
       </c>
@@ -595,6 +635,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>19.98</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>49.53 %</t>
         </is>
       </c>
@@ -613,6 +658,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>28.17</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>38.87 %</t>
         </is>
       </c>
@@ -631,6 +681,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>48.18</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>47.83 %</t>
         </is>
       </c>
@@ -649,6 +704,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>-20.16</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>-13.05 %</t>
         </is>
       </c>
@@ -667,6 +727,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>2.76</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>5.72 %</t>
         </is>
       </c>
@@ -685,6 +750,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>12.61</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>27.29 %</t>
         </is>
       </c>
@@ -703,6 +773,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>38.05</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>70.33 %</t>
         </is>
       </c>
@@ -721,6 +796,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>80.90</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>33.51 %</t>
         </is>
       </c>
@@ -739,6 +819,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>27.45</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>86.24 %</t>
         </is>
       </c>
@@ -757,6 +842,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>23.92</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>17.61 %</t>
         </is>
       </c>
@@ -775,6 +865,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>9.97</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>11.85 %</t>
         </is>
       </c>
@@ -793,6 +888,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>10.87</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>99.63 %</t>
         </is>
       </c>
@@ -811,6 +911,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>-5.27</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>-16.75 %</t>
         </is>
       </c>
@@ -829,6 +934,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>62.03</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>103.14 %</t>
         </is>
       </c>
@@ -847,6 +957,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>-6.06</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>-20.41 %</t>
         </is>
       </c>
@@ -865,6 +980,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>-4.85</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>-8.40 %</t>
         </is>
       </c>
@@ -883,6 +1003,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>117.60</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>79.46 %</t>
         </is>
       </c>
@@ -900,6 +1025,11 @@
         <v>41.9</v>
       </c>
       <c r="D26" t="inlineStr">
+        <is>
+          <t>19.29</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>85.32 %</t>
         </is>

</xml_diff>

<commit_message>
Shows quantity in final file but mixing USD-T and UL
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Difference</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Total gain (%)</t>
         </is>
@@ -470,16 +475,21 @@
         <v>120.355</v>
       </c>
       <c r="C2" t="n">
-        <v>172.4286</v>
+        <v>178.9503</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>52.07</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>43.27 %</t>
+          <t>58.60</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>48.69 %</t>
         </is>
       </c>
     </row>
@@ -493,545 +503,637 @@
         <v>84.59999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>103.72</v>
+        <v>112.68</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>19.12</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>22.60 %</t>
+          <t>28.08</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>33.19 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AXP</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>79.84</v>
+        <v>147.95</v>
       </c>
       <c r="C4" t="n">
-        <v>159.41</v>
+        <v>203.55</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>79.57</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>99.66 %</t>
+          <t>55.60</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>37.58 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BA</t>
+          <t>BAC</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>147.95</v>
+        <v>28.9725</v>
       </c>
       <c r="C5" t="n">
-        <v>193.29</v>
+        <v>44.5664</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>45.34</t>
+          <t>6.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>30.65 %</t>
+          <t>15.59</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>53.82 %</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BAC</t>
+          <t>BTC-USD</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28.9725</v>
+        <v>44833</v>
       </c>
       <c r="C6" t="n">
-        <v>44.126775</v>
+        <v>47649.16</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15.15</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>52.31 %</t>
+          <t>2816.16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>6.28 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BTC-USD</t>
+          <t>CEZ.PR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>44833</v>
+        <v>719</v>
       </c>
       <c r="C7" t="n">
-        <v>46465.625</v>
+        <v>827</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1632.62</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.64 %</t>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>15.02 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CEZ.PR</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>719</v>
+        <v>40.33</v>
       </c>
       <c r="C8" t="n">
-        <v>806</v>
+        <v>63.8</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>87.00</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12.10 %</t>
+          <t>23.47</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>58.19 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>CVS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>40.33</v>
+        <v>72.48</v>
       </c>
       <c r="C9" t="n">
-        <v>60.305</v>
+        <v>104</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>19.98</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>49.53 %</t>
+          <t>31.52</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>43.49 %</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>72.48</v>
+        <v>100.74</v>
       </c>
       <c r="C10" t="n">
-        <v>100.65</v>
+        <v>156.355</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>28.17</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>38.87 %</t>
+          <t>55.61</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>55.21 %</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>GRMN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>100.74</v>
+        <v>154.5</v>
       </c>
       <c r="C11" t="n">
-        <v>148.92</v>
+        <v>137.2</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>48.18</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>47.83 %</t>
+          <t>-17.30</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-11.20 %</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GRMN</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>154.5</v>
+        <v>48.15666666666667</v>
       </c>
       <c r="C12" t="n">
-        <v>134.335</v>
+        <v>52.01333333333333</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>-20.16</t>
+          <t>4.00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-13.05 %</t>
+          <t>3.86</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>8.01 %</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48.15666666666667</v>
+        <v>46.22666666666667</v>
       </c>
       <c r="C13" t="n">
-        <v>50.91333333333333</v>
+        <v>58.94333333333334</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.76</t>
+          <t>5.00</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>5.72 %</t>
+          <t>12.72</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>27.51 %</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>MONET.PR</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>46.22666666666667</v>
+        <v>54.1</v>
       </c>
       <c r="C14" t="n">
-        <v>58.84</v>
+        <v>93.75</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>12.61</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>27.29 %</t>
+          <t>39.65</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>73.29 %</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MONET.PR</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>54.1</v>
+        <v>241.44</v>
       </c>
       <c r="C15" t="n">
-        <v>92.15000000000001</v>
+        <v>340.94</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>38.05</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>70.33 %</t>
+          <t>99.50</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>41.21 %</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>241.44</v>
+        <v>31.83</v>
       </c>
       <c r="C16" t="n">
-        <v>322.339</v>
+        <v>58.59</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>80.90</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>33.51 %</t>
+          <t>26.76</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>84.07 %</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>31.83</v>
+        <v>135.8</v>
       </c>
       <c r="C17" t="n">
-        <v>59.28</v>
+        <v>162.8956</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>27.45</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>86.24 %</t>
+          <t>27.10</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>19.95 %</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>135.8</v>
+        <v>84.155</v>
       </c>
       <c r="C18" t="n">
-        <v>159.72</v>
+        <v>94.55</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>23.92</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>17.61 %</t>
+          <t>10.39</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>12.35 %</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>SAVE</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>84.155</v>
+        <v>10.91</v>
       </c>
       <c r="C19" t="n">
-        <v>94.13</v>
+        <v>22.14</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>9.97</t>
+          <t>3.00</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>11.85 %</t>
+          <t>11.23</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>102.93 %</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SAVE</t>
+          <t>SHLS</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10.91</v>
+        <v>31.435</v>
       </c>
       <c r="C20" t="n">
-        <v>21.78</v>
+        <v>24.78</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10.87</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>99.63 %</t>
+          <t>-6.66</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-21.17 %</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SHLS</t>
+          <t>SONY</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>31.435</v>
+        <v>60.14</v>
       </c>
       <c r="C21" t="n">
-        <v>26.17</v>
+        <v>126.36</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>-5.27</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-16.75 %</t>
+          <t>66.22</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>110.11 %</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SONY</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>60.14</v>
+        <v>29.67</v>
       </c>
       <c r="C22" t="n">
-        <v>122.1677</v>
+        <v>24.795</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>62.03</t>
+          <t>1.00</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>103.14 %</t>
+          <t>-4.88</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-16.43 %</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>UL</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>29.67</v>
+        <v>57.77</v>
       </c>
       <c r="C23" t="n">
-        <v>23.615</v>
+        <v>53.63</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>-6.06</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-20.41 %</t>
+          <t>-4.14</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-7.17 %</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>UL</t>
+          <t>VOW.DE</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>57.77</v>
+        <v>148</v>
       </c>
       <c r="C24" t="n">
-        <v>52.92</v>
+        <v>258.4</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>-4.85</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-8.40 %</t>
+          <t>110.40</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>74.59 %</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>VOW.DE</t>
+          <t>XPEV</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>148</v>
+        <v>22.61</v>
       </c>
       <c r="C25" t="n">
-        <v>265.6</v>
+        <v>49.17</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>117.60</t>
+          <t>2.00</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>79.46 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>XPEV</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>22.61</v>
-      </c>
-      <c r="C26" t="n">
-        <v>41.9</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>19.29</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>85.32 %</t>
+          <t>26.56</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>117.47 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Stock_reporter_no_panda mixing BTC/USD and UL quantity
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -479,7 +479,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -507,7 +507,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.00</t>
+          <t>6.000000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -580,560 +580,560 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BTC-USD</t>
+          <t>CEZ.PR</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>44833</v>
+        <v>719</v>
       </c>
       <c r="C6" t="n">
-        <v>47649.16</v>
+        <v>827</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2816.16</t>
+          <t>108.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>6.28 %</t>
+          <t>15.02 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CEZ.PR</t>
+          <t>CSCO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>719</v>
+        <v>40.33</v>
       </c>
       <c r="C7" t="n">
-        <v>827</v>
+        <v>63.8</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>3.000000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>108.00</t>
+          <t>23.47</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>15.02 %</t>
+          <t>58.19 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CSCO</t>
+          <t>CVS</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>40.33</v>
+        <v>72.48</v>
       </c>
       <c r="C8" t="n">
-        <v>63.8</v>
+        <v>104</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>3.000000</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>23.47</t>
+          <t>31.52</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>58.19 %</t>
+          <t>43.49 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>DIS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>72.48</v>
+        <v>100.74</v>
       </c>
       <c r="C9" t="n">
-        <v>104</v>
+        <v>156.355</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>31.52</t>
+          <t>55.61</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>43.49 %</t>
+          <t>55.21 %</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DIS</t>
+          <t>GRMN</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100.74</v>
+        <v>154.5</v>
       </c>
       <c r="C10" t="n">
-        <v>156.355</v>
+        <v>137.2</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>55.61</t>
+          <t>-17.30</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>55.21 %</t>
+          <t>-11.20 %</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GRMN</t>
+          <t>INTC</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>154.5</v>
+        <v>48.15666666666667</v>
       </c>
       <c r="C11" t="n">
-        <v>137.2</v>
+        <v>52.01333333333333</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>4.000000</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-17.30</t>
+          <t>3.86</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-11.20 %</t>
+          <t>8.01 %</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>INTC</t>
+          <t>KO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>48.15666666666667</v>
+        <v>46.22666666666667</v>
       </c>
       <c r="C12" t="n">
-        <v>52.01333333333333</v>
+        <v>58.94333333333334</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>4.00</t>
+          <t>5.000000</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.86</t>
+          <t>12.72</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>8.01 %</t>
+          <t>27.51 %</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KO</t>
+          <t>MONET.PR</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>46.22666666666667</v>
+        <v>54.1</v>
       </c>
       <c r="C13" t="n">
-        <v>58.94333333333334</v>
+        <v>93.75</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12.72</t>
+          <t>39.65</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>27.51 %</t>
+          <t>73.29 %</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MONET.PR</t>
+          <t>MSFT</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>54.1</v>
+        <v>241.44</v>
       </c>
       <c r="C14" t="n">
-        <v>93.75</v>
+        <v>340.94</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>39.65</t>
+          <t>99.50</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>73.29 %</t>
+          <t>41.21 %</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>PFE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>241.44</v>
+        <v>31.83</v>
       </c>
       <c r="C15" t="n">
-        <v>340.94</v>
+        <v>58.59</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>99.50</t>
+          <t>26.76</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>41.21 %</t>
+          <t>84.07 %</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PFE</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>31.83</v>
+        <v>135.8</v>
       </c>
       <c r="C16" t="n">
-        <v>58.59</v>
+        <v>162.8956</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>26.76</t>
+          <t>27.10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>84.07 %</t>
+          <t>19.95 %</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>PM</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>135.8</v>
+        <v>84.155</v>
       </c>
       <c r="C17" t="n">
-        <v>162.8956</v>
+        <v>94.55</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>3.000000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>27.10</t>
+          <t>10.39</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>19.95 %</t>
+          <t>12.35 %</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PM</t>
+          <t>SAVE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>84.155</v>
+        <v>10.91</v>
       </c>
       <c r="C18" t="n">
-        <v>94.55</v>
+        <v>22.14</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>3.000000</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>10.39</t>
+          <t>11.23</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>12.35 %</t>
+          <t>102.93 %</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SAVE</t>
+          <t>SHLS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10.91</v>
+        <v>31.435</v>
       </c>
       <c r="C19" t="n">
-        <v>22.14</v>
+        <v>24.78</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>11.23</t>
+          <t>-6.66</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>102.93 %</t>
+          <t>-21.17 %</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SHLS</t>
+          <t>SONY</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>31.435</v>
+        <v>60.14</v>
       </c>
       <c r="C20" t="n">
-        <v>24.78</v>
+        <v>126.36</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-6.66</t>
+          <t>66.22</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-21.17 %</t>
+          <t>110.11 %</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SONY</t>
+          <t>T</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>60.14</v>
+        <v>29.67</v>
       </c>
       <c r="C21" t="n">
-        <v>126.36</v>
+        <v>24.795</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>66.22</t>
+          <t>-4.88</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>110.11 %</t>
+          <t>-16.43 %</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>UL</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>29.67</v>
+        <v>57.77</v>
       </c>
       <c r="C22" t="n">
-        <v>24.795</v>
+        <v>53.63</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.00</t>
+          <t>0.029997</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-4.88</t>
+          <t>-4.14</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>-16.43 %</t>
+          <t>-7.17 %</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>UL</t>
+          <t>VOW.DE</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>57.77</v>
+        <v>148</v>
       </c>
       <c r="C23" t="n">
-        <v>53.63</v>
+        <v>258.4</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-4.14</t>
+          <t>110.40</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-7.17 %</t>
+          <t>74.59 %</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>VOW.DE</t>
+          <t>XPEV</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>148</v>
+        <v>22.61</v>
       </c>
       <c r="C24" t="n">
-        <v>258.4</v>
+        <v>49.17</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>110.40</t>
+          <t>26.56</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>74.59 %</t>
+          <t>117.47 %</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>XPEV</t>
+          <t>xxx</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>22.61</v>
+        <v>44833</v>
       </c>
       <c r="C25" t="n">
-        <v>49.17</v>
+        <v>47649.16</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2.00</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>26.56</t>
+          <t>2816.16</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>117.47 %</t>
+          <t>6.28 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added total absolute and relative gains/looses
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,6 +461,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Total gain</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Total gain (%)</t>
         </is>
       </c>
@@ -468,42 +473,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BTC-USD</t>
+          <t>AAPL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>44833</v>
+        <v>120.355</v>
       </c>
       <c r="C2" t="n">
-        <v>47629.92</v>
+        <v>177.145</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.029997</t>
+          <t>2.000000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2796.92</t>
+          <t>56.79</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6.24 %</t>
+          <t>113.58</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>47.19 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CEZ.PR</t>
+          <t>AIR.PA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>719</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>827</v>
+        <v>112.68</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -512,26 +522,31 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>108.00</t>
+          <t>28.08</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>15.02 %</t>
+          <t>28.08</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>33.19 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GRMN</t>
+          <t>AXP</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>154.5</v>
+        <v>79.84</v>
       </c>
       <c r="C4" t="n">
-        <v>136.71</v>
+        <v>164.52</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -540,96 +555,743 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-17.79</t>
+          <t>84.68</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-11.51 %</t>
+          <t>84.68</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>106.06 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>BA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>135.8</v>
+        <v>147.95</v>
       </c>
       <c r="C5" t="n">
-        <v>160.24</v>
+        <v>204.03</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2.000000</t>
+          <t>1.000000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>24.44</t>
+          <t>56.08</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>18.00 %</t>
+          <t>56.08</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>37.90 %</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TTWO</t>
+          <t>BAC</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>167.82</v>
+        <v>28.9725</v>
       </c>
       <c r="C6" t="n">
-        <v>180.83</v>
+        <v>44.455</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.000000</t>
+          <t>6.000000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>13.01</t>
+          <t>15.48</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>7.75 %</t>
+          <t>92.90</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>53.44 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>BTC-USD</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>44833</v>
+      </c>
+      <c r="C7" t="n">
+        <v>47281.67</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.029997</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2448.67</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>73.45</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>5.46 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CEZ.PR</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>719</v>
+      </c>
+      <c r="C8" t="n">
+        <v>827</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>15.02 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>40.33</v>
+      </c>
+      <c r="C9" t="n">
+        <v>62.245</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2.000000</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>21.91</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>43.83</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>54.34 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>72.48</v>
+      </c>
+      <c r="C10" t="n">
+        <v>101.45</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>5.000000</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>28.97</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>144.85</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>39.97 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DIS</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>100.74</v>
+      </c>
+      <c r="C11" t="n">
+        <v>153.8394</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>53.10</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>53.10</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>52.71 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GRMN</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>154.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>136.71</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-17.79</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-17.79</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-11.51 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>48.15666666666667</v>
+      </c>
+      <c r="C13" t="n">
+        <v>51.51500000000001</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>3.36</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>13.43</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>6.97 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>46.22666666666667</v>
+      </c>
+      <c r="C14" t="n">
+        <v>58.04</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>4.000000</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>11.81</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>47.25</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>25.56 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MONET.PR</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>92.8</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2.000000</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>38.70</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>77.40</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>71.53 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>241.44</v>
+      </c>
+      <c r="C16" t="n">
+        <v>339.32</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>97.88</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>97.88</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>40.54 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>31.83</v>
+      </c>
+      <c r="C17" t="n">
+        <v>58.335</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>26.51</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>26.51</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>83.27 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="C18" t="n">
+        <v>162.77</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2.000000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>26.97</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>53.94</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>19.86 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>PM</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>84.155</v>
+      </c>
+      <c r="C19" t="n">
+        <v>93.0911</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2.000000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>8.94</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>17.87</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>10.62 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SAVE</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>10.91</v>
+      </c>
+      <c r="C20" t="n">
+        <v>22.82</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3.000000</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>11.91</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>35.73</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>109.17 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SHLS</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>31.435</v>
+      </c>
+      <c r="C21" t="n">
+        <v>24.73</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3.000000</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>-6.71</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-20.12</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-21.33 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SONY</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>60.14</v>
+      </c>
+      <c r="C22" t="n">
+        <v>125.92</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>65.78</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>65.78</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>109.38 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>29.67</v>
+      </c>
+      <c r="C23" t="n">
+        <v>24.855</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>-4.82</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-4.82</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-16.23 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TTWO</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>167.82</v>
+      </c>
+      <c r="C24" t="n">
+        <v>180.83</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>13.01</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>13.01</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>7.75 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>UL</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B25" t="n">
         <v>57.77</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C25" t="n">
         <v>53.58</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>2.000000</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>-4.19</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-8.38</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>-7.25 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>VOW.DE</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>148</v>
+      </c>
+      <c r="C26" t="n">
+        <v>264</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>1.000000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>116.00</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>116.00</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>78.38 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added total gain in %
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Difference</t>
+          <t>Current Difference</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -467,6 +467,11 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total gain (%)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>P/L (%)</t>
         </is>
       </c>
     </row>
@@ -480,7 +485,7 @@
         <v>120.355</v>
       </c>
       <c r="C2" t="n">
-        <v>177.145</v>
+        <v>182.01</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -489,17 +494,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>56.79</t>
+          <t>61.65</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>113.58</t>
+          <t>123.31</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>47.19 %</t>
+          <t>51.23 %</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -513,7 +523,7 @@
         <v>84.59999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>112.68</v>
+        <v>116.14</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -522,17 +532,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>28.08</t>
+          <t>31.54</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>28.08</t>
+          <t>31.54</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>33.19 %</t>
+          <t>37.28 %</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -546,7 +561,7 @@
         <v>79.84</v>
       </c>
       <c r="C4" t="n">
-        <v>164.52</v>
+        <v>168.21</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -555,17 +570,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>84.68</t>
+          <t>88.37</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>84.68</t>
+          <t>88.37</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>106.06 %</t>
+          <t>110.68 %</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -579,7 +599,7 @@
         <v>147.95</v>
       </c>
       <c r="C5" t="n">
-        <v>204.03</v>
+        <v>207.87</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -588,17 +608,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>56.08</t>
+          <t>59.92</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>56.08</t>
+          <t>59.92</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>37.90 %</t>
+          <t>40.50 %</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -612,7 +637,7 @@
         <v>28.9725</v>
       </c>
       <c r="C6" t="n">
-        <v>44.455</v>
+        <v>46.18</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -621,17 +646,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>15.48</t>
+          <t>17.21</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>92.90</t>
+          <t>103.24</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>53.44 %</t>
+          <t>59.39 %</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -645,7 +675,7 @@
         <v>44833</v>
       </c>
       <c r="C7" t="n">
-        <v>47281.67</v>
+        <v>45897.945</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -654,17 +684,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2448.67</t>
+          <t>1064.94</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>73.45</t>
+          <t>31.95</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5.46 %</t>
+          <t>2.38 %</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -678,7 +713,7 @@
         <v>719</v>
       </c>
       <c r="C8" t="n">
-        <v>827</v>
+        <v>806.5</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -687,17 +722,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>108.00</t>
+          <t>87.50</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>108.00</t>
+          <t>87.50</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>15.02 %</t>
+          <t>12.17 %</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -711,7 +751,7 @@
         <v>40.33</v>
       </c>
       <c r="C9" t="n">
-        <v>62.245</v>
+        <v>63.16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -720,17 +760,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>21.91</t>
+          <t>22.83</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>43.83</t>
+          <t>45.66</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>54.34 %</t>
+          <t>56.61 %</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -744,7 +789,7 @@
         <v>72.48</v>
       </c>
       <c r="C10" t="n">
-        <v>101.45</v>
+        <v>104.15</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -753,17 +798,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>28.97</t>
+          <t>31.67</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>144.85</t>
+          <t>158.35</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>39.97 %</t>
+          <t>43.69 %</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -777,7 +827,7 @@
         <v>100.74</v>
       </c>
       <c r="C11" t="n">
-        <v>153.8394</v>
+        <v>156.73</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -786,17 +836,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>53.10</t>
+          <t>55.99</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>53.10</t>
+          <t>55.99</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>52.71 %</t>
+          <t>55.58 %</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -810,7 +865,7 @@
         <v>154.5</v>
       </c>
       <c r="C12" t="n">
-        <v>136.71</v>
+        <v>133.85</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -819,17 +874,22 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-17.79</t>
+          <t>-20.65</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-17.79</t>
+          <t>-20.65</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-11.51 %</t>
+          <t>-13.37 %</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -843,7 +903,7 @@
         <v>48.15666666666667</v>
       </c>
       <c r="C13" t="n">
-        <v>51.51500000000001</v>
+        <v>53.21</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -852,17 +912,22 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3.36</t>
+          <t>5.05</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>13.43</t>
+          <t>20.21</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6.97 %</t>
+          <t>10.49 %</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -876,7 +941,7 @@
         <v>46.22666666666667</v>
       </c>
       <c r="C14" t="n">
-        <v>58.04</v>
+        <v>59.29499999999999</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -885,17 +950,22 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>11.81</t>
+          <t>13.07</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>47.25</t>
+          <t>52.27</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>25.56 %</t>
+          <t>28.27 %</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -909,7 +979,7 @@
         <v>54.1</v>
       </c>
       <c r="C15" t="n">
-        <v>92.8</v>
+        <v>94.09999999999999</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -918,17 +988,22 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>38.70</t>
+          <t>40.00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>77.40</t>
+          <t>80.00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>71.53 %</t>
+          <t>73.94 %</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -942,7 +1017,7 @@
         <v>241.44</v>
       </c>
       <c r="C16" t="n">
-        <v>339.32</v>
+        <v>334.75</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -951,17 +1026,22 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>97.88</t>
+          <t>93.31</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>97.88</t>
+          <t>93.31</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>40.54 %</t>
+          <t>38.65 %</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -975,7 +1055,7 @@
         <v>31.83</v>
       </c>
       <c r="C17" t="n">
-        <v>58.335</v>
+        <v>56.66</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -984,17 +1064,22 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>26.51</t>
+          <t>24.83</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>26.51</t>
+          <t>24.83</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>83.27 %</t>
+          <t>78.01 %</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1008,7 +1093,7 @@
         <v>135.8</v>
       </c>
       <c r="C18" t="n">
-        <v>162.77</v>
+        <v>162.89</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1017,17 +1102,22 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>26.97</t>
+          <t>27.09</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>53.94</t>
+          <t>54.18</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>19.86 %</t>
+          <t>19.95 %</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1131,7 @@
         <v>84.155</v>
       </c>
       <c r="C19" t="n">
-        <v>93.0911</v>
+        <v>95.76000000000001</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1050,17 +1140,22 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>8.94</t>
+          <t>11.61</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>17.87</t>
+          <t>23.21</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>10.62 %</t>
+          <t>13.79 %</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1169,7 @@
         <v>10.91</v>
       </c>
       <c r="C20" t="n">
-        <v>22.82</v>
+        <v>22.48</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1083,17 +1178,22 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>11.91</t>
+          <t>11.57</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>35.73</t>
+          <t>34.71</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>109.17 %</t>
+          <t>106.05 %</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1207,7 @@
         <v>31.435</v>
       </c>
       <c r="C21" t="n">
-        <v>24.73</v>
+        <v>23.84</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1116,17 +1216,22 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-6.71</t>
+          <t>-7.60</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>-20.12</t>
+          <t>-22.79</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-21.33 %</t>
+          <t>-24.16 %</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1245,7 @@
         <v>60.14</v>
       </c>
       <c r="C22" t="n">
-        <v>125.92</v>
+        <v>126.2599</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1149,17 +1254,22 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>65.78</t>
+          <t>66.12</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>65.78</t>
+          <t>66.12</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>109.38 %</t>
+          <t>109.94 %</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1173,7 +1283,7 @@
         <v>29.67</v>
       </c>
       <c r="C23" t="n">
-        <v>24.855</v>
+        <v>25.43</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1182,17 +1292,22 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-4.82</t>
+          <t>-4.24</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-4.82</t>
+          <t>-4.24</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-16.23 %</t>
+          <t>-14.29 %</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1321,7 @@
         <v>167.82</v>
       </c>
       <c r="C24" t="n">
-        <v>180.83</v>
+        <v>178.61</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1215,17 +1330,22 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>13.01</t>
+          <t>10.79</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>13.01</t>
+          <t>10.79</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>7.75 %</t>
+          <t>6.43 %</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1359,7 @@
         <v>57.77</v>
       </c>
       <c r="C25" t="n">
-        <v>53.58</v>
+        <v>54.06</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1248,17 +1368,22 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-4.19</t>
+          <t>-3.71</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>-8.38</t>
+          <t>-7.42</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>-7.25 %</t>
+          <t>-6.42 %</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1397,7 @@
         <v>148</v>
       </c>
       <c r="C26" t="n">
-        <v>264</v>
+        <v>265.6</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1281,17 +1406,22 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>116.00</t>
+          <t>117.60</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>116.00</t>
+          <t>117.60</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>78.38 %</t>
+          <t>79.46 %</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>26.53 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added function for counting number of rows and merging the rows
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +50,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +75,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,9 +438,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -471,7 +484,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>P/L (%)</t>
+          <t>P/L</t>
         </is>
       </c>
     </row>
@@ -509,7 +522,8 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>26.53 %</t>
+          <t>P/L 
+ 26.53%</t>
         </is>
       </c>
     </row>
@@ -545,11 +559,6 @@
           <t>37.28 %</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -583,11 +592,6 @@
           <t>110.68 %</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -621,11 +625,6 @@
           <t>40.50 %</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -659,11 +658,6 @@
           <t>59.39 %</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -697,11 +691,6 @@
           <t>2.38 %</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -735,11 +724,6 @@
           <t>12.17 %</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -773,11 +757,6 @@
           <t>56.61 %</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -811,11 +790,6 @@
           <t>43.69 %</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -849,11 +823,6 @@
           <t>55.58 %</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -887,11 +856,6 @@
           <t>-13.37 %</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -925,11 +889,6 @@
           <t>10.49 %</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -963,11 +922,6 @@
           <t>28.27 %</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1001,11 +955,6 @@
           <t>73.94 %</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1039,11 +988,6 @@
           <t>38.65 %</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1077,11 +1021,6 @@
           <t>78.01 %</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1115,11 +1054,6 @@
           <t>19.95 %</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1153,11 +1087,6 @@
           <t>13.79 %</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1191,11 +1120,6 @@
           <t>106.05 %</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1229,11 +1153,6 @@
           <t>-24.16 %</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1267,11 +1186,6 @@
           <t>109.94 %</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1305,11 +1219,6 @@
           <t>-14.29 %</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1343,11 +1252,6 @@
           <t>6.43 %</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1381,11 +1285,6 @@
           <t>-6.42 %</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1419,13 +1318,14 @@
           <t>79.46 %</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>26.53 %</t>
-        </is>
-      </c>
-    </row>
+    </row>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="1">
+    <mergeCell ref="H2:H29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Counts total P/L in percent and converts .xlsx to .html
</commit_message>
<xml_diff>
--- a/Stock_final.xlsx
+++ b/Stock_final.xlsx
@@ -522,7 +522,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>P/L  3.93%</t>
+          <t>P/L  12.52%</t>
         </is>
       </c>
     </row>
@@ -668,7 +668,7 @@
         <v>44833</v>
       </c>
       <c r="C7" t="n">
-        <v>35142.504</v>
+        <v>35256.523</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -677,17 +677,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-9690.50</t>
+          <t>-9576.48</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-290.69</t>
+          <t>-287.27</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-21.61 %</t>
+          <t>-21.36 %</t>
         </is>
       </c>
     </row>

</xml_diff>